<commit_message>
Fix scan_example to work with the latest version of scan, add task to push necessary forms, fix zip file script
</commit_message>
<xml_diff>
--- a/app/config/tables/scan_example/forms/scan_example/scan_example.xlsx
+++ b/app/config/tables/scan_example/forms/scan_example/scan_example.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\toolsuite\app-designer\app\config\tables\scan_example\forms\scan_example\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="22503" yWindow="2919" windowWidth="25606" windowHeight="16560" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="3620" yWindow="7380" windowWidth="44760" windowHeight="16240" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="97">
   <si>
     <t>clause</t>
   </si>
@@ -261,9 +256,6 @@
     <t>array</t>
   </si>
   <si>
-    <t>["address","address_image0_contentType","address_image0_uriFragment","comments","comments_image0_contentType","comments_image0_uriFragment","fri_chores","fri_chores_image0_contentType","fri_chores_image0_uriFragment","mon_chores","mon_chores_image0_contentType","mon_chores_image0_uriFragment","name","name_image0_contentType","name_image0_uriFragment","qrcode","qrcode_image0_contentType","qrcode_image0_uriFragment","roomNum","roomNum_image0_contentType","roomNum_image0_uriFragment","sat_chores","sat_chores_image0_contentType","sat_chores_image0_uriFragment","scan_output_directory","stay","stay_image0_contentType","stay_image0_uriFragment","sun_chores","sun_chores_image0_contentType","sun_chores_image0_uriFragment","thurs_chores","thurs_chores_image0_contentType","thurs_chores_image0_uriFragment","tues_chores","tues_chores_image0_contentType","tues_chores_image0_uriFragment","wed_chores","wed_chores_image0_contentType","wed_chores_image0_uriFragment"]</t>
-  </si>
-  <si>
     <t>defaultViewType</t>
   </si>
   <si>
@@ -283,6 +275,45 @@
   </si>
   <si>
     <t>config/tables/scan_example/html/scan_example_detail.html</t>
+  </si>
+  <si>
+    <t>elementType</t>
+  </si>
+  <si>
+    <t>properties.uriFragment.type</t>
+  </si>
+  <si>
+    <t>properties.contentType.type</t>
+  </si>
+  <si>
+    <t>properties.contentType.default</t>
+  </si>
+  <si>
+    <t>raw</t>
+  </si>
+  <si>
+    <t>object</t>
+  </si>
+  <si>
+    <t>rowpath</t>
+  </si>
+  <si>
+    <t>mimeUri</t>
+  </si>
+  <si>
+    <t>application/json</t>
+  </si>
+  <si>
+    <t>properties.uriFragment.elementType</t>
+  </si>
+  <si>
+    <t>properties.contentType.elementType</t>
+  </si>
+  <si>
+    <t>mimeType</t>
+  </si>
+  <si>
+    <t>["address","address_image0_contentType","address_image0_uriFragment","comments","comments_image0_contentType","comments_image0_uriFragment","fri_chores","fri_chores_image0_contentType","fri_chores_image0_uriFragment","mon_chores","mon_chores_image0_contentType","mon_chores_image0_uriFragment","name","name_image0_contentType","name_image0_uriFragment","qrcode","qrcode_image0_contentType","qrcode_image0_uriFragment","raw","raw_contentType","raw_uriFragment","roomNum","roomNum_image0_contentType","roomNum_image0_uriFragment","sat_chores","sat_chores_image0_contentType","sat_chores_image0_uriFragment","scan_output_directory","stay","stay_image0_contentType","stay_image0_uriFragment","sun_chores","sun_chores_image0_contentType","sun_chores_image0_uriFragment","thurs_chores","thurs_chores_image0_contentType","thurs_chores_image0_uriFragment","tues_chores","tues_chores_image0_contentType","tues_chores_image0_uriFragment","wed_chores","wed_chores_image0_contentType","wed_chores_image0_uriFragment"]</t>
   </si>
 </sst>
 </file>
@@ -331,17 +362,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -682,17 +725,17 @@
   <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" customWidth="1"/>
-    <col min="4" max="4" width="31.109375" customWidth="1"/>
+    <col min="4" max="4" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -712,12 +755,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -728,7 +771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -739,17 +782,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -760,7 +803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -771,17 +814,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -792,7 +835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -803,17 +846,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6">
       <c r="B15" t="s">
         <v>7</v>
       </c>
@@ -824,7 +867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6">
       <c r="B16" t="s">
         <v>12</v>
       </c>
@@ -835,17 +878,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6">
       <c r="B19" t="s">
         <v>7</v>
       </c>
@@ -856,7 +899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6">
       <c r="B20" t="s">
         <v>8</v>
       </c>
@@ -867,17 +910,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6">
       <c r="B23" t="s">
         <v>7</v>
       </c>
@@ -888,7 +931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6">
       <c r="B24" t="s">
         <v>22</v>
       </c>
@@ -902,17 +945,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6">
       <c r="B27" t="s">
         <v>7</v>
       </c>
@@ -923,7 +966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6">
       <c r="B28" t="s">
         <v>22</v>
       </c>
@@ -937,17 +980,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6">
       <c r="B31" t="s">
         <v>7</v>
       </c>
@@ -958,7 +1001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6">
       <c r="B32" t="s">
         <v>22</v>
       </c>
@@ -972,17 +1015,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6">
       <c r="B35" t="s">
         <v>7</v>
       </c>
@@ -993,7 +1036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6">
       <c r="B36" t="s">
         <v>22</v>
       </c>
@@ -1007,17 +1050,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6">
       <c r="B39" t="s">
         <v>7</v>
       </c>
@@ -1028,7 +1071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6">
       <c r="B40" t="s">
         <v>22</v>
       </c>
@@ -1042,17 +1085,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6">
       <c r="B43" t="s">
         <v>7</v>
       </c>
@@ -1063,7 +1106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6">
       <c r="B44" t="s">
         <v>22</v>
       </c>
@@ -1077,17 +1120,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6">
       <c r="B47" t="s">
         <v>7</v>
       </c>
@@ -1098,7 +1141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6">
       <c r="B48" t="s">
         <v>22</v>
       </c>
@@ -1112,17 +1155,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6">
       <c r="B51" t="s">
         <v>7</v>
       </c>
@@ -1133,7 +1176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6">
       <c r="B52" t="s">
         <v>8</v>
       </c>
@@ -1144,7 +1187,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>11</v>
       </c>
@@ -1168,14 +1211,14 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
     <col min="3" max="3" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -1186,7 +1229,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1197,7 +1240,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1208,7 +1251,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1219,7 +1262,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1242,23 +1285,47 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="25.83203125" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" customWidth="1"/>
+    <col min="6" max="7" width="34" customWidth="1"/>
+    <col min="8" max="8" width="29.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -1266,8 +1333,35 @@
         <v>39</v>
       </c>
     </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H3" t="s">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1284,12 +1378,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -1300,7 +1394,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -1308,7 +1402,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1316,7 +1410,7 @@
         <v>20140810</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -1339,17 +1433,17 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
     <col min="4" max="5" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>70</v>
       </c>
@@ -1366,7 +1460,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -1380,10 +1474,10 @@
         <v>76</v>
       </c>
       <c r="E2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -1391,16 +1485,16 @@
         <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
         <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -1408,16 +1502,16 @@
         <v>74</v>
       </c>
       <c r="C4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" t="s">
         <v>80</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>81</v>
       </c>
-      <c r="E4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -1425,16 +1519,21 @@
         <v>74</v>
       </c>
       <c r="C5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" t="s">
         <v>83</v>
-      </c>
-      <c r="D5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
presumably the updates for things that really matter
</commit_message>
<xml_diff>
--- a/app/config/tables/scan_example/forms/scan_example/scan_example.xlsx
+++ b/app/config/tables/scan_example/forms/scan_example/scan_example.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\toolsuite\app-designer\app\config\tables\scan_example\forms\scan_example\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="22503" yWindow="2919" windowWidth="25606" windowHeight="16560" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="3620" yWindow="7380" windowWidth="44760" windowHeight="16240" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="97">
   <si>
     <t>clause</t>
   </si>
@@ -261,9 +256,6 @@
     <t>array</t>
   </si>
   <si>
-    <t>["address","address_image0_contentType","address_image0_uriFragment","comments","comments_image0_contentType","comments_image0_uriFragment","fri_chores","fri_chores_image0_contentType","fri_chores_image0_uriFragment","mon_chores","mon_chores_image0_contentType","mon_chores_image0_uriFragment","name","name_image0_contentType","name_image0_uriFragment","qrcode","qrcode_image0_contentType","qrcode_image0_uriFragment","roomNum","roomNum_image0_contentType","roomNum_image0_uriFragment","sat_chores","sat_chores_image0_contentType","sat_chores_image0_uriFragment","scan_output_directory","stay","stay_image0_contentType","stay_image0_uriFragment","sun_chores","sun_chores_image0_contentType","sun_chores_image0_uriFragment","thurs_chores","thurs_chores_image0_contentType","thurs_chores_image0_uriFragment","tues_chores","tues_chores_image0_contentType","tues_chores_image0_uriFragment","wed_chores","wed_chores_image0_contentType","wed_chores_image0_uriFragment"]</t>
-  </si>
-  <si>
     <t>defaultViewType</t>
   </si>
   <si>
@@ -283,6 +275,45 @@
   </si>
   <si>
     <t>config/tables/scan_example/html/scan_example_detail.html</t>
+  </si>
+  <si>
+    <t>elementType</t>
+  </si>
+  <si>
+    <t>properties.uriFragment.type</t>
+  </si>
+  <si>
+    <t>properties.contentType.type</t>
+  </si>
+  <si>
+    <t>properties.contentType.default</t>
+  </si>
+  <si>
+    <t>raw</t>
+  </si>
+  <si>
+    <t>object</t>
+  </si>
+  <si>
+    <t>rowpath</t>
+  </si>
+  <si>
+    <t>mimeUri</t>
+  </si>
+  <si>
+    <t>application/json</t>
+  </si>
+  <si>
+    <t>properties.uriFragment.elementType</t>
+  </si>
+  <si>
+    <t>properties.contentType.elementType</t>
+  </si>
+  <si>
+    <t>mimeType</t>
+  </si>
+  <si>
+    <t>["address","address_image0_contentType","address_image0_uriFragment","comments","comments_image0_contentType","comments_image0_uriFragment","fri_chores","fri_chores_image0_contentType","fri_chores_image0_uriFragment","mon_chores","mon_chores_image0_contentType","mon_chores_image0_uriFragment","name","name_image0_contentType","name_image0_uriFragment","qrcode","qrcode_image0_contentType","qrcode_image0_uriFragment","raw","raw_contentType","raw_uriFragment","roomNum","roomNum_image0_contentType","roomNum_image0_uriFragment","sat_chores","sat_chores_image0_contentType","sat_chores_image0_uriFragment","scan_output_directory","stay","stay_image0_contentType","stay_image0_uriFragment","sun_chores","sun_chores_image0_contentType","sun_chores_image0_uriFragment","thurs_chores","thurs_chores_image0_contentType","thurs_chores_image0_uriFragment","tues_chores","tues_chores_image0_contentType","tues_chores_image0_uriFragment","wed_chores","wed_chores_image0_contentType","wed_chores_image0_uriFragment"]</t>
   </si>
 </sst>
 </file>
@@ -331,17 +362,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -682,17 +725,17 @@
   <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" customWidth="1"/>
-    <col min="4" max="4" width="31.109375" customWidth="1"/>
+    <col min="4" max="4" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -712,12 +755,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -728,7 +771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -739,17 +782,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -760,7 +803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -771,17 +814,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -792,7 +835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -803,17 +846,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6">
       <c r="B15" t="s">
         <v>7</v>
       </c>
@@ -824,7 +867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6">
       <c r="B16" t="s">
         <v>12</v>
       </c>
@@ -835,17 +878,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6">
       <c r="B19" t="s">
         <v>7</v>
       </c>
@@ -856,7 +899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6">
       <c r="B20" t="s">
         <v>8</v>
       </c>
@@ -867,17 +910,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6">
       <c r="B23" t="s">
         <v>7</v>
       </c>
@@ -888,7 +931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6">
       <c r="B24" t="s">
         <v>22</v>
       </c>
@@ -902,17 +945,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6">
       <c r="B27" t="s">
         <v>7</v>
       </c>
@@ -923,7 +966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6">
       <c r="B28" t="s">
         <v>22</v>
       </c>
@@ -937,17 +980,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6">
       <c r="B31" t="s">
         <v>7</v>
       </c>
@@ -958,7 +1001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6">
       <c r="B32" t="s">
         <v>22</v>
       </c>
@@ -972,17 +1015,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6">
       <c r="B35" t="s">
         <v>7</v>
       </c>
@@ -993,7 +1036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6">
       <c r="B36" t="s">
         <v>22</v>
       </c>
@@ -1007,17 +1050,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6">
       <c r="B39" t="s">
         <v>7</v>
       </c>
@@ -1028,7 +1071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6">
       <c r="B40" t="s">
         <v>22</v>
       </c>
@@ -1042,17 +1085,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6">
       <c r="B43" t="s">
         <v>7</v>
       </c>
@@ -1063,7 +1106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6">
       <c r="B44" t="s">
         <v>22</v>
       </c>
@@ -1077,17 +1120,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6">
       <c r="B47" t="s">
         <v>7</v>
       </c>
@@ -1098,7 +1141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6">
       <c r="B48" t="s">
         <v>22</v>
       </c>
@@ -1112,17 +1155,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6">
       <c r="B51" t="s">
         <v>7</v>
       </c>
@@ -1133,7 +1176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6">
       <c r="B52" t="s">
         <v>8</v>
       </c>
@@ -1144,7 +1187,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>11</v>
       </c>
@@ -1168,14 +1211,14 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
     <col min="3" max="3" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -1186,7 +1229,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1197,7 +1240,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1208,7 +1251,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1219,7 +1262,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1242,23 +1285,47 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="25.83203125" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" customWidth="1"/>
+    <col min="6" max="7" width="34" customWidth="1"/>
+    <col min="8" max="8" width="29.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -1266,8 +1333,35 @@
         <v>39</v>
       </c>
     </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H3" t="s">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1284,12 +1378,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -1300,7 +1394,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -1308,7 +1402,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1316,7 +1410,7 @@
         <v>20140810</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -1339,17 +1433,17 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
     <col min="4" max="5" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>70</v>
       </c>
@@ -1366,7 +1460,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -1380,10 +1474,10 @@
         <v>76</v>
       </c>
       <c r="E2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -1391,16 +1485,16 @@
         <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
         <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -1408,16 +1502,16 @@
         <v>74</v>
       </c>
       <c r="C4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" t="s">
         <v>80</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>81</v>
       </c>
-      <c r="E4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -1425,16 +1519,21 @@
         <v>74</v>
       </c>
       <c r="C5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" t="s">
         <v>83</v>
-      </c>
-      <c r="D5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>